<commit_message>
Update cell value code  and small change in order number fetching using getAttribute
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -72,7 +72,7 @@
     <t>flgkhleiw</t>
   </si>
   <si>
-    <t>sownd</t>
+    <t>P57O1SFIGJ</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
         <v>9</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -495,7 +495,7 @@
         <v>345</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>